<commit_message>
simple bot test ok
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deluc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAE55F4-4FD9-489A-9F30-85C9B1212371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E37476-5E94-4843-8B0D-B9A390E1C6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E23EB597-9E83-4E60-A1B4-48DC3E59E872}"/>
   </bookViews>
   <sheets>
     <sheet name="Contatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Telefone</t>
   </si>
@@ -50,16 +50,136 @@
     <t>Vinicius Simulacro</t>
   </si>
   <si>
-    <t>+5511981267978</t>
-  </si>
-  <si>
-    <t>Amanda LuzCena</t>
-  </si>
-  <si>
-    <t>+5511976244914</t>
-  </si>
-  <si>
-    <t>Aninha Bibi</t>
+    <t>+5513991892211</t>
+  </si>
+  <si>
+    <t>aloha bar</t>
+  </si>
+  <si>
+    <t>+5561995672332</t>
+  </si>
+  <si>
+    <t>Porks</t>
+  </si>
+  <si>
+    <t>+5513974226875</t>
+  </si>
+  <si>
+    <t>Beco Bar</t>
+  </si>
+  <si>
+    <t>+5513998027988</t>
+  </si>
+  <si>
+    <t>Maleh</t>
+  </si>
+  <si>
+    <t>+5513996000859</t>
+  </si>
+  <si>
+    <t>Resenhas</t>
+  </si>
+  <si>
+    <t>+5513996672625</t>
+  </si>
+  <si>
+    <t>Barzin da praia</t>
+  </si>
+  <si>
+    <t>Avenisdas Bar e espeto</t>
+  </si>
+  <si>
+    <t>+5513991328222</t>
+  </si>
+  <si>
+    <t>Confraria do forte</t>
+  </si>
+  <si>
+    <t>Quiosque 7</t>
+  </si>
+  <si>
+    <t>+5513991342205</t>
+  </si>
+  <si>
+    <t>Vixe Bar</t>
+  </si>
+  <si>
+    <t>Matilde Bar</t>
+  </si>
+  <si>
+    <t>Capitão Bar</t>
+  </si>
+  <si>
+    <t>+5513991037423</t>
+  </si>
+  <si>
+    <t>+5513974019871</t>
+  </si>
+  <si>
+    <t>+5513981356526</t>
+  </si>
+  <si>
+    <t>neco's bar</t>
+  </si>
+  <si>
+    <t>+5513996935710</t>
+  </si>
+  <si>
+    <t>+5513981840830</t>
+  </si>
+  <si>
+    <t>+5513997005002</t>
+  </si>
+  <si>
+    <t>wall street hamb</t>
+  </si>
+  <si>
+    <t>+5513996009483</t>
+  </si>
+  <si>
+    <t>Nabarca sushi</t>
+  </si>
+  <si>
+    <t>+5513991302000</t>
+  </si>
+  <si>
+    <t>Elo Adega e Tabaca</t>
+  </si>
+  <si>
+    <t>+5513991705555</t>
+  </si>
+  <si>
+    <t>Baroni Bar</t>
+  </si>
+  <si>
+    <t>+5513974098864</t>
+  </si>
+  <si>
+    <t>Pink Bar</t>
+  </si>
+  <si>
+    <t>+551333295300</t>
+  </si>
+  <si>
+    <t>Santo Canto</t>
+  </si>
+  <si>
+    <t>+551335916484</t>
+  </si>
+  <si>
+    <t>Gaucho Mallet Gril</t>
+  </si>
+  <si>
+    <t>+5513988659250</t>
+  </si>
+  <si>
+    <t>Espetos Japa e Cia</t>
+  </si>
+  <si>
+    <t>+5513997529370</t>
+  </si>
+  <si>
+    <t>Bar se7e</t>
   </si>
 </sst>
 </file>
@@ -412,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125FD6DB-6AB9-49E9-8BF0-557C9D7640BD}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +576,166 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>